<commit_message>
changed all lines to 8 mil min width
</commit_message>
<xml_diff>
--- a/wing-actuator/board/act-drive1-bom-digikey.xlsx
+++ b/wing-actuator/board/act-drive1-bom-digikey.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
   <si>
     <t>Qty</t>
   </si>
@@ -348,9 +348,6 @@
     <t>D2, D3, D4, D5, D6, D7, D8, D9, D11, D12, D13, D14, D15, D16, D17, D18,D19,D20, D21, D22, D23, D24, D25, D26, D27, D30, D31, D32, D33, D34, D35, D36, D38, D39, D40</t>
   </si>
   <si>
-    <t>D1, D10, D19, D28</t>
-  </si>
-  <si>
     <t>R5, R18, R1, R9, R13</t>
   </si>
   <si>
@@ -364,6 +361,15 @@
   </si>
   <si>
     <t>DMN60H080DS-7DICT-ND</t>
+  </si>
+  <si>
+    <t>D1, D10, D19, D28, D41</t>
+  </si>
+  <si>
+    <t>H3CCS-1618M-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Position Cable Assembly Rectangular Socket to Socket 1.50' </t>
   </si>
 </sst>
 </file>
@@ -861,13 +867,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1189,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:XFD36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,7 +1266,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
@@ -1266,7 +1278,7 @@
         <v>53</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>54</v>
@@ -1298,12 +1310,81 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
@@ -1312,13 +1393,13 @@
         <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1326,7 +1407,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -1335,448 +1416,391 @@
         <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>1</v>
       </c>
-      <c r="B16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D17" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="E17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G19" t="s">
-        <v>28</v>
+      <c r="G17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="G22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>6</v>
-      </c>
-      <c r="B26" t="s">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>75</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G28" t="s">
-        <v>80</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="D34" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G34" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
-      <c r="B37" t="s">
-        <v>90</v>
-      </c>
       <c r="C37" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>4</v>
-      </c>
-      <c r="B38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" t="s">
-        <v>94</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>4</v>
-      </c>
-      <c r="B39" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" t="s">
-        <v>98</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>3</v>
-      </c>
-      <c r="B40" t="s">
-        <v>101</v>
-      </c>
-      <c r="C40" t="s">
-        <v>101</v>
-      </c>
-      <c r="D40" t="s">
-        <v>102</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>3</v>
-      </c>
-      <c r="C41" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>19</v>
-      </c>
-      <c r="D42" t="s">
-        <v>20</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F42" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
b.o.m. for actuator drive board
</commit_message>
<xml_diff>
--- a/wing-actuator/board/act-drive1-bom-digikey.xlsx
+++ b/wing-actuator/board/act-drive1-bom-digikey.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="118">
   <si>
     <t>Qty</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t xml:space="preserve">16 Position Cable Assembly Rectangular Socket to Socket 1.50' </t>
+  </si>
+  <si>
+    <t>SV1P, SV2P</t>
   </si>
 </sst>
 </file>
@@ -1203,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,6 +1639,9 @@
       <c r="A27">
         <v>2</v>
       </c>
+      <c r="E27" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="F27" s="1" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
updated labels on PCB
</commit_message>
<xml_diff>
--- a/wing-actuator/board/act-drive1-bom-digikey.xlsx
+++ b/wing-actuator/board/act-drive1-bom-digikey.xlsx
@@ -14,7 +14,10 @@
   <sheets>
     <sheet name="act-drive1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'act-drive1'!$A$1:$G$35</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1204,20 +1207,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1615,203 +1622,204 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" t="s">
+        <v>87</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28">
+        <v>89</v>
+      </c>
+      <c r="G27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>1</v>
       </c>
-      <c r="B28" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>4</v>
       </c>
-      <c r="B29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D33" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>4</v>
-      </c>
-      <c r="B34" t="s">
-        <v>97</v>
+        <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>99</v>
+        <v>14</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>3</v>
-      </c>
-      <c r="B35" t="s">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>20</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>103</v>
+        <v>21</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>19</v>
-      </c>
-      <c r="D37" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F37" s="1" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="87" fitToHeight="2" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>